<commit_message>
Remove needless imports on org.dozer
</commit_message>
<xml_diff>
--- a/org.openl.rules.mapping.dev.test/src/test/resources/org/openl/rules/mapping/conditions/FieldMappingConditionsUsageOrderTest.xlsx
+++ b/org.openl.rules.mapping.dev.test/src/test/resources/org/openl/rules/mapping/conditions/FieldMappingConditionsUsageOrderTest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="24735" windowHeight="11955"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>classA</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>dontMap</t>
-  </si>
-  <si>
-    <t>org.dozer</t>
   </si>
   <si>
     <t>Method boolean map(Object src, Object dest)</t>
@@ -116,8 +113,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,7 +161,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -208,17 +205,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -242,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -260,7 +246,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -270,10 +255,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -282,6 +267,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -360,6 +350,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -394,6 +385,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -569,14 +561,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C7:H20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C7:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
@@ -585,95 +577,109 @@
     <col min="7" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="3:8">
-      <c r="C7" s="10" t="s">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="10"/>
-    </row>
-    <row r="8" spans="3:8">
-      <c r="C8" s="11" t="s">
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="3:8">
-      <c r="C9" s="12"/>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="11"/>
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="3:8">
-      <c r="C10" s="12"/>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="11"/>
       <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="3:8">
-      <c r="C11" s="12"/>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="11"/>
       <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="3:8">
-      <c r="C12" s="12"/>
-      <c r="D12" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8">
-      <c r="C15" s="8" t="s">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="3:8">
-      <c r="C16" s="2" t="s">
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="3:8" ht="60" customHeight="1">
-      <c r="C17" s="3" t="s">
+    <row r="16" spans="3:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="3:8">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>21</v>
       </c>
@@ -681,10 +687,10 @@
         <v>19</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G18" t="s">
         <v>25</v>
@@ -693,7 +699,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="3:8">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>21</v>
       </c>
@@ -701,37 +707,17 @@
         <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8">
-      <c r="C20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C14:H14"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="C8:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -739,36 +725,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B4:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="82.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:2">
-      <c r="B8" s="6" t="s">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2">
-      <c r="B12" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2">
-      <c r="B13" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>